<commit_message>
Add sales and administration expenses spreadsheet for IPADE MEDE MTY 2026
</commit_message>
<xml_diff>
--- a/Procurement/EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx
+++ b/Procurement/EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0dc407a335d7300f/Documentos/GitHub/BusinessSim/Procurement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1500" documentId="11_300C377E292435E26BC7E9727970CF20457E0EE2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A51A8C1-61FE-4FF3-AFE2-EE723C353007}"/>
+  <xr:revisionPtr revIDLastSave="1502" documentId="11_300C377E292435E26BC7E9727970CF20457E0EE2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE1D1FAB-CC15-4C89-A572-260930471AF7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BUYING_PLAN_FINAL" sheetId="18" r:id="rId1"/>
@@ -1540,11 +1540,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3545,18 +3545,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
@@ -3573,18 +3573,18 @@
       <c r="J2" s="82"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="79" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -3757,18 +3757,18 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -3979,16 +3979,16 @@
       <c r="H1" s="88"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="79" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="53" t="s">
@@ -4055,16 +4055,16 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="79" t="s">
         <v>202</v>
       </c>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="53" t="s">
@@ -4195,12 +4195,12 @@
       <c r="J2" s="92"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="79" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
@@ -4247,18 +4247,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="79" t="s">
         <v>220</v>
       </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
     </row>
     <row r="13" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
@@ -4364,16 +4364,16 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="79" t="s">
         <v>228</v>
       </c>
-      <c r="B18" s="77"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
-      <c r="G18" s="77"/>
-      <c r="H18" s="77"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
@@ -6410,48 +6410,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="78" t="s">
         <v>233</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="79" t="s">
         <v>234</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
@@ -6643,18 +6643,18 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="79" t="s">
         <v>238</v>
       </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
@@ -6812,18 +6812,18 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="79" t="s">
         <v>240</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="77"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="77"/>
-      <c r="J19" s="77"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
@@ -7025,12 +7025,12 @@
       <c r="A27" s="93"/>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="77" t="s">
+      <c r="A28" s="79" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="77"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="77"/>
+      <c r="B28" s="79"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="79"/>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="53" t="s">
@@ -7131,13 +7131,13 @@
       <c r="E2" s="83"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="79" t="s">
         <v>254</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -7271,13 +7271,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="79" t="s">
         <v>260</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -7457,13 +7457,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="79" t="s">
         <v>261</v>
       </c>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
@@ -7673,13 +7673,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
@@ -7691,13 +7691,13 @@
       <c r="E2" s="82"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="79" t="s">
         <v>264</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -7923,14 +7923,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>268</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
@@ -7943,14 +7943,14 @@
       <c r="F2" s="82"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="79" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -8322,16 +8322,16 @@
       <c r="H2" s="82"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="79" t="s">
         <v>290</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -9235,15 +9235,15 @@
       <c r="G2" s="82"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="79" t="s">
         <v>293</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -15118,8 +15118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15132,49 +15132,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
+      <c r="A1" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -15242,12 +15242,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
@@ -15376,12 +15376,12 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
@@ -15510,12 +15510,12 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="77"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
@@ -15670,12 +15670,12 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="77" t="s">
+      <c r="A45" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="77"/>
-      <c r="C45" s="77"/>
-      <c r="D45" s="77"/>
+      <c r="B45" s="79"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="79"/>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
@@ -15813,13 +15813,13 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="77" t="s">
+      <c r="A57" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="77"/>
-      <c r="C57" s="77"/>
-      <c r="D57" s="77"/>
-      <c r="E57" s="77"/>
+      <c r="B57" s="79"/>
+      <c r="C57" s="79"/>
+      <c r="D57" s="79"/>
+      <c r="E57" s="79"/>
     </row>
     <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
@@ -15878,15 +15878,15 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="77" t="s">
+      <c r="A64" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="77"/>
-      <c r="C64" s="77"/>
-      <c r="D64" s="77"/>
-      <c r="E64" s="77"/>
-      <c r="F64" s="77"/>
-      <c r="G64" s="77"/>
+      <c r="B64" s="79"/>
+      <c r="C64" s="79"/>
+      <c r="D64" s="79"/>
+      <c r="E64" s="79"/>
+      <c r="F64" s="79"/>
+      <c r="G64" s="79"/>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
@@ -15977,15 +15977,15 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="77" t="s">
+      <c r="A72" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="B72" s="77"/>
-      <c r="C72" s="77"/>
-      <c r="D72" s="77"/>
-      <c r="E72" s="77"/>
-      <c r="F72" s="77"/>
-      <c r="G72" s="77"/>
+      <c r="B72" s="79"/>
+      <c r="C72" s="79"/>
+      <c r="D72" s="79"/>
+      <c r="E72" s="79"/>
+      <c r="F72" s="79"/>
+      <c r="G72" s="79"/>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
@@ -16076,12 +16076,12 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="77" t="s">
+      <c r="A80" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="77"/>
-      <c r="C80" s="77"/>
-      <c r="D80" s="77"/>
+      <c r="B80" s="79"/>
+      <c r="C80" s="79"/>
+      <c r="D80" s="79"/>
     </row>
     <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
@@ -16182,22 +16182,22 @@
       </c>
     </row>
     <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="78" t="s">
+      <c r="A88" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="B88" s="78"/>
-      <c r="C88" s="78"/>
-      <c r="D88" s="78"/>
-      <c r="E88" s="78"/>
+      <c r="B88" s="80"/>
+      <c r="C88" s="80"/>
+      <c r="D88" s="80"/>
+      <c r="E88" s="80"/>
     </row>
     <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="79" t="s">
+      <c r="A89" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="79"/>
-      <c r="C89" s="79"/>
-      <c r="D89" s="79"/>
-      <c r="E89" s="79"/>
+      <c r="B89" s="81"/>
+      <c r="C89" s="81"/>
+      <c r="D89" s="81"/>
+      <c r="E89" s="81"/>
     </row>
     <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
@@ -16482,11 +16482,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A80:D80"/>
     <mergeCell ref="A88:E88"/>
     <mergeCell ref="A89:E89"/>
@@ -16495,6 +16490,11 @@
     <mergeCell ref="A57:E57"/>
     <mergeCell ref="A64:G64"/>
     <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -16525,20 +16525,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
@@ -17025,7 +17025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
@@ -17043,19 +17043,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
@@ -17088,19 +17088,19 @@
       <c r="K3" s="85"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -17272,19 +17272,19 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="77"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="79"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -17456,19 +17456,19 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="77"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -17640,19 +17640,19 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -17824,19 +17824,19 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="77"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="77"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="77"/>
-      <c r="J29" s="77"/>
-      <c r="K29" s="77"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="79"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
@@ -18008,19 +18008,19 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="77" t="s">
+      <c r="A35" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="77"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="77"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
@@ -18192,19 +18192,19 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="77" t="s">
+      <c r="A41" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="77"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="77"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="77"/>
-      <c r="I41" s="77"/>
-      <c r="J41" s="77"/>
-      <c r="K41" s="77"/>
+      <c r="B41" s="79"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="79"/>
+      <c r="F41" s="79"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="79"/>
+      <c r="I41" s="79"/>
+      <c r="J41" s="79"/>
+      <c r="K41" s="79"/>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
@@ -18376,19 +18376,19 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="77" t="s">
+      <c r="A47" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="77"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="77"/>
-      <c r="G47" s="77"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="77"/>
-      <c r="J47" s="77"/>
-      <c r="K47" s="77"/>
+      <c r="B47" s="79"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="79"/>
+      <c r="E47" s="79"/>
+      <c r="F47" s="79"/>
+      <c r="G47" s="79"/>
+      <c r="H47" s="79"/>
+      <c r="I47" s="79"/>
+      <c r="J47" s="79"/>
+      <c r="K47" s="79"/>
     </row>
     <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
@@ -18560,18 +18560,18 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="78" t="s">
+      <c r="A53" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="B53" s="78"/>
-      <c r="C53" s="78"/>
-      <c r="D53" s="78"/>
-      <c r="E53" s="78"/>
-      <c r="F53" s="78"/>
-      <c r="G53" s="78"/>
-      <c r="H53" s="78"/>
-      <c r="I53" s="78"/>
-      <c r="J53" s="78"/>
+      <c r="B53" s="80"/>
+      <c r="C53" s="80"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="80"/>
+      <c r="F53" s="80"/>
+      <c r="G53" s="80"/>
+      <c r="H53" s="80"/>
+      <c r="I53" s="80"/>
+      <c r="J53" s="80"/>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
@@ -18935,11 +18935,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A11:K11"/>
     <mergeCell ref="A47:K47"/>
     <mergeCell ref="A53:J53"/>
     <mergeCell ref="A17:K17"/>
@@ -18947,6 +18942,11 @@
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A35:K35"/>
     <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A11:K11"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:I10">
     <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
@@ -19021,20 +19021,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
@@ -19069,18 +19069,18 @@
       <c r="L3" s="87"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
     </row>
     <row r="6" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
@@ -19349,20 +19349,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="79" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="77"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="77"/>
-      <c r="L16" s="77"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
     </row>
     <row r="17" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
@@ -20094,14 +20094,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
@@ -20367,20 +20367,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
@@ -20615,14 +20615,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
@@ -20812,14 +20812,14 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="79" t="s">
         <v>170</v>
       </c>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">

</xml_diff>